<commit_message>
Working with CSV and EXCEL Data
</commit_message>
<xml_diff>
--- a/PythonSkillDev/sample.xlsx
+++ b/PythonSkillDev/sample.xlsx
@@ -136,7 +136,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>BAR CHART</a:t>
+              <a:t>LINE CHART</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -163,7 +163,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$A$1:$A$10</f>
+              <f>'Sheet'!$A$1:$A$5</f>
             </numRef>
           </val>
         </ser>
@@ -563,47 +563,47 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>